<commit_message>
Update 2. Space Game IPO_Table.xlsx
</commit_message>
<xml_diff>
--- a/Publications/2. Space Game IPO_Table.xlsx
+++ b/Publications/2. Space Game IPO_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\OneDrive\Documents\MSSA Homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsant\Documents\GitHub\BountyCollector\Publications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39227406-6026-4538-8A53-5AF1432E67B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8390BE-F76F-4C79-8262-57D9926065FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3CE7D408-B133-492C-A10E-57F5D16D2E22}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="15390" windowHeight="9585" xr2:uid="{3CE7D408-B133-492C-A10E-57F5D16D2E22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,22 +516,22 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.796875" customWidth="1"/>
+    <col min="6" max="6" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:6" ht="15.75" x14ac:dyDescent="0.45">
       <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
@@ -553,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D5" s="8"/>
       <c r="E5" s="5" t="s">
         <v>7</v>
@@ -562,14 +562,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:6" ht="15.75" x14ac:dyDescent="0.45">
       <c r="D8" s="3" t="s">
         <v>0</v>
       </c>
@@ -580,7 +580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
@@ -591,7 +591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D10" s="8"/>
       <c r="E10" s="2" t="s">
         <v>5</v>

</xml_diff>